<commit_message>
Deletes old Http and Ping excel files
</commit_message>
<xml_diff>
--- a/A02/MocoPA02Java/dataPa2/excelfiles/status-01.xlsx
+++ b/A02/MocoPA02Java/dataPa2/excelfiles/status-01.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>SystemTime</t>
   </si>
@@ -160,6 +160,14 @@
         <v>1.041489509E9</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.465993371E9</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.041489509E9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -219,6 +227,29 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.465993371E9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -278,6 +309,29 @@
         <v>1024.0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.465993371E9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="n">
+        <v>38076.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1024.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -337,6 +391,29 @@
         <v>25</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.465993371E9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1024.0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -419,6 +496,52 @@
         <v>283210.0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1.465993371E9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1024.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1.465993371E9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1024.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>283210.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>